<commit_message>
minor bug fixes to data gridview column names and addition of extra brands for pants and jackets
</commit_message>
<xml_diff>
--- a/References/InvTemplate.xlsx
+++ b/References/InvTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebas\Desktop\Work\InventorySystem\References\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1E5FE57-B8FE-4B72-87E0-18E73FEAD153}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E8BF2D7-2C75-4ED7-9F95-106378236C9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-18307" yWindow="-5767" windowWidth="18400" windowHeight="13120" activeTab="2" xr2:uid="{340EB9D4-906C-4284-A45B-2D9B12819D14}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="3" xr2:uid="{340EB9D4-906C-4284-A45B-2D9B12819D14}"/>
   </bookViews>
   <sheets>
     <sheet name="Jackets" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2400" uniqueCount="447">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2401" uniqueCount="449">
   <si>
     <t>LOCATION</t>
   </si>
@@ -1383,6 +1383,12 @@
   </si>
   <si>
     <t>Material</t>
+  </si>
+  <si>
+    <t>Size</t>
+  </si>
+  <si>
+    <t>DueDate</t>
   </si>
 </sst>
 </file>
@@ -10376,7 +10382,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AF3C3E2-32FC-45E8-BAEF-9C786CFA4436}">
   <dimension ref="A1:H211"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -12945,10 +12951,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE89F8C7-8911-48C0-979A-AA5614134282}">
-  <dimension ref="A1:H211"/>
+  <dimension ref="A1:I211"/>
   <sheetViews>
-    <sheetView topLeftCell="A183" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection sqref="A1:H211"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12959,11 +12965,12 @@
     <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.21875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.44140625" customWidth="1"/>
+    <col min="8" max="8" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="61.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>6</v>
       </c>
@@ -12974,8 +12981,9 @@
       <c r="F1" s="5"/>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
-    </row>
-    <row r="2" spans="1:8" ht="25.8" x14ac:dyDescent="0.3">
+      <c r="I1" s="5"/>
+    </row>
+    <row r="2" spans="1:9" ht="25.8" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>16</v>
       </c>
@@ -12995,13 +13003,16 @@
         <v>17</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>18</v>
+        <v>447</v>
       </c>
       <c r="H2" s="10" t="s">
+        <v>448</v>
+      </c>
+      <c r="I2" s="10" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -13009,11 +13020,12 @@
       <c r="E3" s="3"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
-      <c r="H3" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H3" s="1"/>
+      <c r="I3" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -13021,11 +13033,12 @@
       <c r="E4" s="3"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
-      <c r="H4" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H4" s="1"/>
+      <c r="I4" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -13033,11 +13046,12 @@
       <c r="E5" s="3"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
-      <c r="H5" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H5" s="1"/>
+      <c r="I5" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
@@ -13045,11 +13059,12 @@
       <c r="E6" s="8"/>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
-      <c r="H6" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H6" s="7"/>
+      <c r="I6" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -13057,11 +13072,12 @@
       <c r="E7" s="2"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
-      <c r="H7" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H7" s="1"/>
+      <c r="I7" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -13069,11 +13085,12 @@
       <c r="E8" s="2"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
-      <c r="H8" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H8" s="1"/>
+      <c r="I8" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -13081,11 +13098,12 @@
       <c r="E9" s="2"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
-      <c r="H9" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H9" s="1"/>
+      <c r="I9" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -13093,11 +13111,12 @@
       <c r="E10" s="2"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
-      <c r="H10" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H10" s="1"/>
+      <c r="I10" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -13105,11 +13124,12 @@
       <c r="E11" s="2"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
-      <c r="H11" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H11" s="1"/>
+      <c r="I11" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -13117,11 +13137,12 @@
       <c r="E12" s="2"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
-      <c r="H12" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H12" s="1"/>
+      <c r="I12" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -13129,11 +13150,12 @@
       <c r="E13" s="2"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
-      <c r="H13" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H13" s="1"/>
+      <c r="I13" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -13141,11 +13163,12 @@
       <c r="E14" s="2"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
-      <c r="H14" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H14" s="1"/>
+      <c r="I14" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -13153,11 +13176,12 @@
       <c r="E15" s="2"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
-      <c r="H15" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H15" s="1"/>
+      <c r="I15" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -13165,11 +13189,12 @@
       <c r="E16" s="2"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
-      <c r="H16" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H16" s="1"/>
+      <c r="I16" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -13177,11 +13202,12 @@
       <c r="E17" s="2"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
-      <c r="H17" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H17" s="1"/>
+      <c r="I17" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -13189,11 +13215,12 @@
       <c r="E18" s="2"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
-      <c r="H18" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H18" s="1"/>
+      <c r="I18" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -13201,11 +13228,12 @@
       <c r="E19" s="2"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
-      <c r="H19" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H19" s="1"/>
+      <c r="I19" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -13213,11 +13241,12 @@
       <c r="E20" s="2"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
-      <c r="H20" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H20" s="1"/>
+      <c r="I20" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -13225,11 +13254,12 @@
       <c r="E21" s="2"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
-      <c r="H21" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H21" s="1"/>
+      <c r="I21" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -13237,11 +13267,12 @@
       <c r="E22" s="2"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
-      <c r="H22" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H22" s="1"/>
+      <c r="I22" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -13249,11 +13280,12 @@
       <c r="E23" s="2"/>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
-      <c r="H23" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H23" s="1"/>
+      <c r="I23" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -13261,11 +13293,12 @@
       <c r="E24" s="2"/>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
-      <c r="H24" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H24" s="1"/>
+      <c r="I24" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -13273,11 +13306,12 @@
       <c r="E25" s="2"/>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
-      <c r="H25" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H25" s="1"/>
+      <c r="I25" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -13285,11 +13319,12 @@
       <c r="E26" s="2"/>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
-      <c r="H26" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H26" s="1"/>
+      <c r="I26" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -13297,11 +13332,12 @@
       <c r="E27" s="2"/>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
-      <c r="H27" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H27" s="1"/>
+      <c r="I27" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -13309,11 +13345,12 @@
       <c r="E28" s="2"/>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
-      <c r="H28" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H28" s="1"/>
+      <c r="I28" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -13321,11 +13358,12 @@
       <c r="E29" s="2"/>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
-      <c r="H29" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H29" s="1"/>
+      <c r="I29" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -13333,11 +13371,12 @@
       <c r="E30" s="2"/>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
-      <c r="H30" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H30" s="1"/>
+      <c r="I30" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -13345,11 +13384,12 @@
       <c r="E31" s="2"/>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
-      <c r="H31" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H31" s="1"/>
+      <c r="I31" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -13357,11 +13397,12 @@
       <c r="E32" s="2"/>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
-      <c r="H32" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H32" s="1"/>
+      <c r="I32" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -13369,11 +13410,12 @@
       <c r="E33" s="2"/>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
-      <c r="H33" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H33" s="1"/>
+      <c r="I33" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -13381,11 +13423,12 @@
       <c r="E34" s="2"/>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
-      <c r="H34" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H34" s="1"/>
+      <c r="I34" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -13393,11 +13436,12 @@
       <c r="E35" s="2"/>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
-      <c r="H35" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H35" s="1"/>
+      <c r="I35" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -13405,11 +13449,12 @@
       <c r="E36" s="2"/>
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
-      <c r="H36" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H36" s="1"/>
+      <c r="I36" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -13417,11 +13462,12 @@
       <c r="E37" s="2"/>
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
-      <c r="H37" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H37" s="1"/>
+      <c r="I37" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -13429,11 +13475,12 @@
       <c r="E38" s="2"/>
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
-      <c r="H38" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H38" s="1"/>
+      <c r="I38" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -13441,11 +13488,12 @@
       <c r="E39" s="2"/>
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
-      <c r="H39" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H39" s="1"/>
+      <c r="I39" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -13453,11 +13501,12 @@
       <c r="E40" s="2"/>
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
-      <c r="H40" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H40" s="1"/>
+      <c r="I40" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -13465,11 +13514,12 @@
       <c r="E41" s="2"/>
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
-      <c r="H41" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H41" s="1"/>
+      <c r="I41" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -13477,11 +13527,12 @@
       <c r="E42" s="2"/>
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
-      <c r="H42" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H42" s="1"/>
+      <c r="I42" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -13489,11 +13540,12 @@
       <c r="E43" s="2"/>
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
-      <c r="H43" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H43" s="1"/>
+      <c r="I43" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -13501,11 +13553,12 @@
       <c r="E44" s="2"/>
       <c r="F44" s="1"/>
       <c r="G44" s="1"/>
-      <c r="H44" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H44" s="1"/>
+      <c r="I44" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -13513,11 +13566,12 @@
       <c r="E45" s="2"/>
       <c r="F45" s="1"/>
       <c r="G45" s="1"/>
-      <c r="H45" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H45" s="1"/>
+      <c r="I45" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -13525,11 +13579,12 @@
       <c r="E46" s="3"/>
       <c r="F46" s="1"/>
       <c r="G46" s="1"/>
-      <c r="H46" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H46" s="1"/>
+      <c r="I46" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -13537,11 +13592,12 @@
       <c r="E47" s="3"/>
       <c r="F47" s="1"/>
       <c r="G47" s="1"/>
-      <c r="H47" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H47" s="1"/>
+      <c r="I47" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -13549,11 +13605,12 @@
       <c r="E48" s="2"/>
       <c r="F48" s="1"/>
       <c r="G48" s="1"/>
-      <c r="H48" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H48" s="1"/>
+      <c r="I48" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -13561,11 +13618,12 @@
       <c r="E49" s="3"/>
       <c r="F49" s="1"/>
       <c r="G49" s="1"/>
-      <c r="H49" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H49" s="1"/>
+      <c r="I49" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -13573,11 +13631,12 @@
       <c r="E50" s="3"/>
       <c r="F50" s="1"/>
       <c r="G50" s="1"/>
-      <c r="H50" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H50" s="1"/>
+      <c r="I50" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -13585,11 +13644,12 @@
       <c r="E51" s="3"/>
       <c r="F51" s="1"/>
       <c r="G51" s="1"/>
-      <c r="H51" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H51" s="1"/>
+      <c r="I51" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -13597,11 +13657,12 @@
       <c r="E52" s="3"/>
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
-      <c r="H52" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H52" s="1"/>
+      <c r="I52" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -13609,11 +13670,12 @@
       <c r="E53" s="3"/>
       <c r="F53" s="1"/>
       <c r="G53" s="1"/>
-      <c r="H53" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H53" s="1"/>
+      <c r="I53" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -13621,11 +13683,12 @@
       <c r="E54" s="3"/>
       <c r="F54" s="1"/>
       <c r="G54" s="1"/>
-      <c r="H54" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H54" s="1"/>
+      <c r="I54" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -13633,11 +13696,12 @@
       <c r="E55" s="3"/>
       <c r="F55" s="1"/>
       <c r="G55" s="1"/>
-      <c r="H55" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H55" s="1"/>
+      <c r="I55" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -13645,11 +13709,12 @@
       <c r="E56" s="3"/>
       <c r="F56" s="1"/>
       <c r="G56" s="1"/>
-      <c r="H56" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H56" s="1"/>
+      <c r="I56" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -13657,11 +13722,12 @@
       <c r="E57" s="3"/>
       <c r="F57" s="1"/>
       <c r="G57" s="1"/>
-      <c r="H57" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H57" s="1"/>
+      <c r="I57" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -13669,11 +13735,12 @@
       <c r="E58" s="3"/>
       <c r="F58" s="1"/>
       <c r="G58" s="1"/>
-      <c r="H58" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H58" s="1"/>
+      <c r="I58" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -13681,11 +13748,12 @@
       <c r="E59" s="3"/>
       <c r="F59" s="1"/>
       <c r="G59" s="1"/>
-      <c r="H59" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H59" s="1"/>
+      <c r="I59" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -13693,11 +13761,12 @@
       <c r="E60" s="1"/>
       <c r="F60" s="1"/>
       <c r="G60" s="1"/>
-      <c r="H60" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H60" s="1"/>
+      <c r="I60" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -13705,11 +13774,12 @@
       <c r="E61" s="3"/>
       <c r="F61" s="1"/>
       <c r="G61" s="1"/>
-      <c r="H61" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H61" s="1"/>
+      <c r="I61" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -13717,11 +13787,12 @@
       <c r="E62" s="3"/>
       <c r="F62" s="1"/>
       <c r="G62" s="1"/>
-      <c r="H62" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H62" s="1"/>
+      <c r="I62" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -13729,11 +13800,12 @@
       <c r="E63" s="3"/>
       <c r="F63" s="1"/>
       <c r="G63" s="1"/>
-      <c r="H63" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H63" s="1"/>
+      <c r="I63" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -13741,11 +13813,12 @@
       <c r="E64" s="2"/>
       <c r="F64" s="1"/>
       <c r="G64" s="1"/>
-      <c r="H64" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H64" s="1"/>
+      <c r="I64" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
@@ -13753,11 +13826,12 @@
       <c r="E65" s="3"/>
       <c r="F65" s="1"/>
       <c r="G65" s="1"/>
-      <c r="H65" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H65" s="1"/>
+      <c r="I65" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -13765,11 +13839,12 @@
       <c r="E66" s="3"/>
       <c r="F66" s="1"/>
       <c r="G66" s="1"/>
-      <c r="H66" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H66" s="1"/>
+      <c r="I66" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -13777,11 +13852,12 @@
       <c r="E67" s="3"/>
       <c r="F67" s="1"/>
       <c r="G67" s="1"/>
-      <c r="H67" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H67" s="1"/>
+      <c r="I67" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
@@ -13789,11 +13865,12 @@
       <c r="E68" s="3"/>
       <c r="F68" s="1"/>
       <c r="G68" s="1"/>
-      <c r="H68" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H68" s="1"/>
+      <c r="I68" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -13801,11 +13878,12 @@
       <c r="E69" s="3"/>
       <c r="F69" s="1"/>
       <c r="G69" s="1"/>
-      <c r="H69" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H69" s="1"/>
+      <c r="I69" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
@@ -13813,11 +13891,12 @@
       <c r="E70" s="3"/>
       <c r="F70" s="1"/>
       <c r="G70" s="1"/>
-      <c r="H70" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H70" s="1"/>
+      <c r="I70" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
@@ -13825,11 +13904,12 @@
       <c r="E71" s="3"/>
       <c r="F71" s="1"/>
       <c r="G71" s="1"/>
-      <c r="H71" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H71" s="1"/>
+      <c r="I71" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
@@ -13837,11 +13917,12 @@
       <c r="E72" s="3"/>
       <c r="F72" s="1"/>
       <c r="G72" s="1"/>
-      <c r="H72" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H72" s="1"/>
+      <c r="I72" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
@@ -13849,11 +13930,12 @@
       <c r="E73" s="3"/>
       <c r="F73" s="1"/>
       <c r="G73" s="1"/>
-      <c r="H73" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H73" s="1"/>
+      <c r="I73" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="7"/>
@@ -13861,11 +13943,12 @@
       <c r="E74" s="3"/>
       <c r="F74" s="1"/>
       <c r="G74" s="1"/>
-      <c r="H74" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H74" s="1"/>
+      <c r="I74" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
@@ -13873,11 +13956,12 @@
       <c r="E75" s="3"/>
       <c r="F75" s="1"/>
       <c r="G75" s="1"/>
-      <c r="H75" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H75" s="1"/>
+      <c r="I75" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
@@ -13885,11 +13969,12 @@
       <c r="E76" s="1"/>
       <c r="F76" s="1"/>
       <c r="G76" s="1"/>
-      <c r="H76" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H76" s="1"/>
+      <c r="I76" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
@@ -13897,11 +13982,12 @@
       <c r="E77" s="2"/>
       <c r="F77" s="1"/>
       <c r="G77" s="1"/>
-      <c r="H77" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H77" s="1"/>
+      <c r="I77" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
@@ -13909,11 +13995,12 @@
       <c r="E78" s="3"/>
       <c r="F78" s="1"/>
       <c r="G78" s="1"/>
-      <c r="H78" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H78" s="1"/>
+      <c r="I78" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
@@ -13921,11 +14008,12 @@
       <c r="E79" s="2"/>
       <c r="F79" s="1"/>
       <c r="G79" s="1"/>
-      <c r="H79" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H79" s="1"/>
+      <c r="I79" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
@@ -13933,11 +14021,12 @@
       <c r="E80" s="3"/>
       <c r="F80" s="1"/>
       <c r="G80" s="1"/>
-      <c r="H80" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H80" s="1"/>
+      <c r="I80" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
@@ -13945,563 +14034,610 @@
       <c r="E81" s="2"/>
       <c r="F81" s="1"/>
       <c r="G81" s="1"/>
-      <c r="H81" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H81" s="1"/>
+      <c r="I81" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A82" s="7"/>
       <c r="B82" s="7"/>
       <c r="C82" s="7"/>
       <c r="D82" s="8"/>
       <c r="E82" s="2"/>
       <c r="F82" s="1"/>
-      <c r="G82" s="6"/>
-      <c r="H82" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G82" s="1"/>
+      <c r="H82" s="6"/>
+      <c r="I82" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A83" s="7"/>
       <c r="B83" s="7"/>
       <c r="C83" s="7"/>
       <c r="D83" s="8"/>
       <c r="E83" s="3"/>
       <c r="F83" s="1"/>
-      <c r="G83" s="6"/>
-      <c r="H83" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G83" s="1"/>
+      <c r="H83" s="6"/>
+      <c r="I83" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A84" s="7"/>
       <c r="B84" s="7"/>
       <c r="C84" s="7"/>
       <c r="D84" s="8"/>
       <c r="E84" s="2"/>
       <c r="F84" s="1"/>
-      <c r="G84" s="6"/>
-      <c r="H84" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G84" s="1"/>
+      <c r="H84" s="6"/>
+      <c r="I84" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A85" s="7"/>
       <c r="B85" s="7"/>
       <c r="C85" s="7"/>
       <c r="D85" s="8"/>
       <c r="E85" s="1"/>
       <c r="F85" s="1"/>
-      <c r="G85" s="6"/>
-      <c r="H85" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G85" s="1"/>
+      <c r="H85" s="6"/>
+      <c r="I85" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A86" s="7"/>
       <c r="B86" s="7"/>
       <c r="C86" s="7"/>
       <c r="D86" s="8"/>
       <c r="E86" s="2"/>
       <c r="F86" s="1"/>
-      <c r="G86" s="6"/>
-      <c r="H86" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G86" s="1"/>
+      <c r="H86" s="6"/>
+      <c r="I86" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A87" s="7"/>
       <c r="B87" s="7"/>
       <c r="C87" s="7"/>
       <c r="D87" s="8"/>
       <c r="E87" s="2"/>
       <c r="F87" s="1"/>
-      <c r="G87" s="6"/>
-      <c r="H87" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G87" s="1"/>
+      <c r="H87" s="6"/>
+      <c r="I87" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A88" s="7"/>
       <c r="B88" s="7"/>
       <c r="C88" s="7"/>
       <c r="D88" s="8"/>
       <c r="E88" s="2"/>
       <c r="F88" s="1"/>
-      <c r="G88" s="6"/>
-      <c r="H88" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G88" s="1"/>
+      <c r="H88" s="6"/>
+      <c r="I88" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A89" s="7"/>
       <c r="B89" s="7"/>
       <c r="C89" s="7"/>
       <c r="D89" s="8"/>
       <c r="E89" s="2"/>
       <c r="F89" s="1"/>
-      <c r="G89" s="6"/>
-      <c r="H89" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G89" s="1"/>
+      <c r="H89" s="6"/>
+      <c r="I89" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A90" s="7"/>
       <c r="B90" s="7"/>
       <c r="C90" s="7"/>
       <c r="D90" s="8"/>
       <c r="E90" s="2"/>
       <c r="F90" s="1"/>
-      <c r="G90" s="6"/>
-      <c r="H90" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G90" s="1"/>
+      <c r="H90" s="6"/>
+      <c r="I90" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A91" s="7"/>
       <c r="B91" s="7"/>
       <c r="C91" s="7"/>
       <c r="D91" s="8"/>
       <c r="E91" s="3"/>
       <c r="F91" s="1"/>
-      <c r="G91" s="6"/>
-      <c r="H91" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G91" s="1"/>
+      <c r="H91" s="6"/>
+      <c r="I91" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A92" s="7"/>
       <c r="B92" s="7"/>
       <c r="C92" s="7"/>
       <c r="D92" s="8"/>
       <c r="E92" s="3"/>
       <c r="F92" s="1"/>
-      <c r="G92" s="6"/>
-      <c r="H92" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G92" s="1"/>
+      <c r="H92" s="6"/>
+      <c r="I92" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A93" s="7"/>
       <c r="B93" s="7"/>
       <c r="C93" s="7"/>
       <c r="D93" s="8"/>
       <c r="E93" s="3"/>
       <c r="F93" s="1"/>
-      <c r="G93" s="6"/>
-      <c r="H93" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G93" s="1"/>
+      <c r="H93" s="6"/>
+      <c r="I93" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A94" s="7"/>
       <c r="B94" s="7"/>
       <c r="C94" s="7"/>
       <c r="D94" s="8"/>
       <c r="E94" s="2"/>
       <c r="F94" s="1"/>
-      <c r="G94" s="6"/>
-      <c r="H94" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G94" s="1"/>
+      <c r="H94" s="6"/>
+      <c r="I94" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A95" s="7"/>
       <c r="B95" s="7"/>
       <c r="C95" s="7"/>
       <c r="D95" s="7"/>
       <c r="E95" s="2"/>
       <c r="F95" s="1"/>
-      <c r="G95" s="6"/>
-      <c r="H95" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G95" s="1"/>
+      <c r="H95" s="6"/>
+      <c r="I95" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A96" s="7"/>
       <c r="B96" s="7"/>
       <c r="C96" s="7"/>
       <c r="D96" s="7"/>
       <c r="E96" s="2"/>
       <c r="F96" s="1"/>
-      <c r="G96" s="6"/>
-      <c r="H96" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G96" s="1"/>
+      <c r="H96" s="6"/>
+      <c r="I96" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A97" s="7"/>
       <c r="B97" s="7"/>
       <c r="C97" s="7"/>
       <c r="D97" s="7"/>
       <c r="E97" s="3"/>
       <c r="F97" s="1"/>
-      <c r="G97" s="6"/>
-      <c r="H97" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G97" s="1"/>
+      <c r="H97" s="6"/>
+      <c r="I97" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A98" s="7"/>
       <c r="B98" s="7"/>
       <c r="C98" s="7"/>
       <c r="D98" s="7"/>
       <c r="E98" s="2"/>
       <c r="F98" s="1"/>
-      <c r="G98" s="6"/>
-      <c r="H98" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G98" s="1"/>
+      <c r="H98" s="6"/>
+      <c r="I98" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A99" s="7"/>
       <c r="B99" s="7"/>
       <c r="C99" s="7"/>
       <c r="D99" s="7"/>
       <c r="E99" s="2"/>
       <c r="F99" s="1"/>
-      <c r="G99" s="6"/>
-      <c r="H99" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G99" s="1"/>
+      <c r="H99" s="6"/>
+      <c r="I99" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A100" s="7"/>
       <c r="B100" s="7"/>
       <c r="C100" s="7"/>
       <c r="D100" s="8"/>
       <c r="E100" s="2"/>
       <c r="F100" s="1"/>
-      <c r="G100" s="6"/>
-      <c r="H100" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G100" s="1"/>
+      <c r="H100" s="6"/>
+      <c r="I100" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A101" s="7"/>
       <c r="B101" s="7"/>
       <c r="C101" s="7"/>
       <c r="D101" s="12"/>
       <c r="E101" s="2"/>
       <c r="F101" s="1"/>
-      <c r="G101" s="6"/>
-      <c r="H101" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G101" s="1"/>
+      <c r="H101" s="6"/>
+      <c r="I101" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A102" s="7"/>
       <c r="B102" s="7"/>
       <c r="C102" s="7"/>
       <c r="D102" s="8"/>
       <c r="E102" s="2"/>
       <c r="F102" s="1"/>
-      <c r="G102" s="6"/>
-      <c r="H102" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G102" s="1"/>
+      <c r="H102" s="6"/>
+      <c r="I102" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A103" s="7"/>
       <c r="B103" s="7"/>
       <c r="C103" s="7"/>
       <c r="D103" s="7"/>
       <c r="E103" s="2"/>
       <c r="F103" s="1"/>
-      <c r="G103" s="6"/>
-      <c r="H103" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G103" s="1"/>
+      <c r="H103" s="6"/>
+      <c r="I103" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A104" s="7"/>
       <c r="B104" s="7"/>
       <c r="C104" s="7"/>
       <c r="D104" s="8"/>
       <c r="E104" s="2"/>
       <c r="F104" s="1"/>
-      <c r="G104" s="6"/>
-      <c r="H104" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G104" s="1"/>
+      <c r="H104" s="6"/>
+      <c r="I104" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A105" s="7"/>
       <c r="B105" s="7"/>
       <c r="C105" s="7"/>
       <c r="D105" s="7"/>
       <c r="E105" s="2"/>
       <c r="F105" s="1"/>
-      <c r="G105" s="6"/>
-      <c r="H105" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G105" s="1"/>
+      <c r="H105" s="6"/>
+      <c r="I105" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A106" s="7"/>
       <c r="B106" s="7"/>
       <c r="C106" s="7"/>
       <c r="D106" s="7"/>
       <c r="E106" s="3"/>
       <c r="F106" s="1"/>
-      <c r="G106" s="6"/>
-      <c r="H106" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G106" s="1"/>
+      <c r="H106" s="6"/>
+      <c r="I106" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A107" s="7"/>
       <c r="B107" s="7"/>
       <c r="C107" s="7"/>
       <c r="D107" s="7"/>
       <c r="E107" s="3"/>
       <c r="F107" s="1"/>
-      <c r="G107" s="6"/>
-      <c r="H107" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G107" s="1"/>
+      <c r="H107" s="6"/>
+      <c r="I107" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A108" s="7"/>
       <c r="B108" s="7"/>
       <c r="C108" s="7"/>
       <c r="D108" s="7"/>
       <c r="E108" s="3"/>
       <c r="F108" s="1"/>
-      <c r="G108" s="6"/>
-      <c r="H108" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G108" s="1"/>
+      <c r="H108" s="6"/>
+      <c r="I108" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A109" s="7"/>
       <c r="B109" s="7"/>
       <c r="C109" s="7"/>
       <c r="D109" s="7"/>
       <c r="E109" s="1"/>
       <c r="F109" s="1"/>
-      <c r="G109" s="6"/>
-      <c r="H109" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G109" s="1"/>
+      <c r="H109" s="6"/>
+      <c r="I109" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A110" s="7"/>
       <c r="B110" s="7"/>
       <c r="C110" s="7"/>
       <c r="D110" s="7"/>
       <c r="E110" s="3"/>
       <c r="F110" s="1"/>
-      <c r="G110" s="6"/>
-      <c r="H110" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G110" s="1"/>
+      <c r="H110" s="6"/>
+      <c r="I110" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A111" s="7"/>
       <c r="B111" s="7"/>
       <c r="C111" s="7"/>
       <c r="D111" s="7"/>
       <c r="E111" s="3"/>
       <c r="F111" s="1"/>
-      <c r="G111" s="6"/>
-      <c r="H111" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G111" s="1"/>
+      <c r="H111" s="6"/>
+      <c r="I111" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A112" s="7"/>
       <c r="B112" s="7"/>
       <c r="C112" s="7"/>
       <c r="D112" s="7"/>
       <c r="E112" s="3"/>
       <c r="F112" s="1"/>
-      <c r="G112" s="6"/>
-      <c r="H112" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G112" s="1"/>
+      <c r="H112" s="6"/>
+      <c r="I112" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A113" s="7"/>
       <c r="B113" s="7"/>
       <c r="C113" s="7"/>
       <c r="D113" s="7"/>
       <c r="E113" s="3"/>
       <c r="F113" s="1"/>
-      <c r="G113" s="6"/>
-      <c r="H113" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G113" s="1"/>
+      <c r="H113" s="6"/>
+      <c r="I113" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A114" s="7"/>
       <c r="B114" s="7"/>
       <c r="C114" s="7"/>
       <c r="D114" s="7"/>
       <c r="E114" s="2"/>
       <c r="F114" s="1"/>
-      <c r="G114" s="6"/>
-      <c r="H114" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G114" s="1"/>
+      <c r="H114" s="6"/>
+      <c r="I114" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A115" s="7"/>
       <c r="B115" s="7"/>
       <c r="C115" s="7"/>
       <c r="D115" s="7"/>
       <c r="E115" s="3"/>
       <c r="F115" s="7"/>
-      <c r="G115" s="6"/>
-      <c r="H115" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G115" s="7"/>
+      <c r="H115" s="6"/>
+      <c r="I115" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A116" s="7"/>
       <c r="B116" s="7"/>
       <c r="C116" s="7"/>
       <c r="D116" s="7"/>
       <c r="E116" s="2"/>
       <c r="F116" s="7"/>
-      <c r="G116" s="6"/>
-      <c r="H116" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G116" s="7"/>
+      <c r="H116" s="6"/>
+      <c r="I116" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A117" s="7"/>
       <c r="B117" s="7"/>
       <c r="C117" s="7"/>
       <c r="D117" s="7"/>
       <c r="E117" s="3"/>
       <c r="F117" s="7"/>
-      <c r="G117" s="6"/>
-      <c r="H117" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G117" s="7"/>
+      <c r="H117" s="6"/>
+      <c r="I117" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A118" s="7"/>
       <c r="B118" s="7"/>
       <c r="C118" s="7"/>
       <c r="D118" s="7"/>
       <c r="E118" s="3"/>
       <c r="F118" s="7"/>
-      <c r="G118" s="6"/>
-      <c r="H118" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G118" s="7"/>
+      <c r="H118" s="6"/>
+      <c r="I118" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A119" s="7"/>
       <c r="B119" s="7"/>
       <c r="C119" s="7"/>
       <c r="D119" s="7"/>
       <c r="E119" s="3"/>
       <c r="F119" s="7"/>
-      <c r="G119" s="6"/>
-      <c r="H119" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G119" s="7"/>
+      <c r="H119" s="6"/>
+      <c r="I119" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A120" s="7"/>
       <c r="B120" s="7"/>
       <c r="C120" s="7"/>
       <c r="D120" s="8"/>
       <c r="E120" s="3"/>
       <c r="F120" s="7"/>
-      <c r="G120" s="6"/>
-      <c r="H120" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G120" s="7"/>
+      <c r="H120" s="6"/>
+      <c r="I120" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A121" s="7"/>
       <c r="B121" s="7"/>
       <c r="C121" s="7"/>
       <c r="D121" s="7"/>
       <c r="E121" s="3"/>
       <c r="F121" s="7"/>
-      <c r="G121" s="6"/>
-      <c r="H121" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G121" s="7"/>
+      <c r="H121" s="6"/>
+      <c r="I121" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A122" s="7"/>
       <c r="B122" s="7"/>
       <c r="C122" s="7"/>
       <c r="D122" s="8"/>
       <c r="E122" s="3"/>
       <c r="F122" s="7"/>
-      <c r="G122" s="6"/>
-      <c r="H122" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G122" s="7"/>
+      <c r="H122" s="6"/>
+      <c r="I122" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A123" s="7"/>
       <c r="B123" s="7"/>
       <c r="C123" s="7"/>
       <c r="D123" s="8"/>
       <c r="E123" s="3"/>
       <c r="F123" s="7"/>
-      <c r="G123" s="6"/>
-      <c r="H123" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G123" s="7"/>
+      <c r="H123" s="6"/>
+      <c r="I123" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A124" s="7"/>
       <c r="B124" s="7"/>
       <c r="C124" s="7"/>
       <c r="D124" s="8"/>
       <c r="E124" s="3"/>
       <c r="F124" s="7"/>
-      <c r="G124" s="6"/>
-      <c r="H124" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G124" s="7"/>
+      <c r="H124" s="6"/>
+      <c r="I124" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A125" s="7"/>
       <c r="B125" s="7"/>
       <c r="C125" s="7"/>
       <c r="D125" s="9"/>
       <c r="E125" s="8"/>
       <c r="F125" s="7"/>
-      <c r="G125" s="6"/>
-      <c r="H125" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G125" s="7"/>
+      <c r="H125" s="6"/>
+      <c r="I125" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A126" s="7"/>
       <c r="B126" s="7"/>
       <c r="C126" s="7"/>
       <c r="D126" s="8"/>
       <c r="E126" s="8"/>
       <c r="F126" s="7"/>
-      <c r="G126" s="6"/>
-      <c r="H126" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G126" s="7"/>
+      <c r="H126" s="6"/>
+      <c r="I126" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="127" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A127" s="7"/>
       <c r="B127" s="7"/>
       <c r="C127" s="7"/>
       <c r="D127" s="8"/>
       <c r="E127" s="8"/>
       <c r="F127" s="7"/>
-      <c r="G127" s="6"/>
-      <c r="H127" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G127" s="7"/>
+      <c r="H127" s="6"/>
+      <c r="I127" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="128" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A128" s="7"/>
       <c r="B128" s="7"/>
       <c r="C128" s="7"/>
@@ -14509,11 +14645,12 @@
       <c r="E128" s="8"/>
       <c r="F128" s="7"/>
       <c r="G128" s="7"/>
-      <c r="H128" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H128" s="7"/>
+      <c r="I128" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="129" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A129" s="7"/>
       <c r="B129" s="7"/>
       <c r="C129" s="7"/>
@@ -14521,23 +14658,25 @@
       <c r="E129" s="8"/>
       <c r="F129" s="7"/>
       <c r="G129" s="7"/>
-      <c r="H129" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H129" s="7"/>
+      <c r="I129" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="130" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A130" s="7"/>
       <c r="B130" s="7"/>
       <c r="C130" s="7"/>
       <c r="D130" s="8"/>
       <c r="E130" s="8"/>
       <c r="F130" s="7"/>
-      <c r="G130" s="6"/>
-      <c r="H130" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G130" s="7"/>
+      <c r="H130" s="6"/>
+      <c r="I130" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="131" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A131" s="7"/>
       <c r="B131" s="7"/>
       <c r="C131" s="7"/>
@@ -14545,11 +14684,12 @@
       <c r="E131" s="8"/>
       <c r="F131" s="7"/>
       <c r="G131" s="7"/>
-      <c r="H131" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H131" s="7"/>
+      <c r="I131" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="132" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A132" s="7"/>
       <c r="B132" s="7"/>
       <c r="C132" s="7"/>
@@ -14557,11 +14697,12 @@
       <c r="E132" s="8"/>
       <c r="F132" s="7"/>
       <c r="G132" s="7"/>
-      <c r="H132" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H132" s="7"/>
+      <c r="I132" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A133" s="7"/>
       <c r="B133" s="7"/>
       <c r="C133" s="7"/>
@@ -14569,11 +14710,12 @@
       <c r="E133" s="8"/>
       <c r="F133" s="7"/>
       <c r="G133" s="7"/>
-      <c r="H133" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H133" s="7"/>
+      <c r="I133" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="134" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A134" s="7"/>
       <c r="B134" s="7"/>
       <c r="C134" s="7"/>
@@ -14581,11 +14723,12 @@
       <c r="E134" s="8"/>
       <c r="F134" s="7"/>
       <c r="G134" s="7"/>
-      <c r="H134" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H134" s="7"/>
+      <c r="I134" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="135" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A135" s="7"/>
       <c r="B135" s="7"/>
       <c r="C135" s="7"/>
@@ -14593,11 +14736,12 @@
       <c r="E135" s="8"/>
       <c r="F135" s="7"/>
       <c r="G135" s="7"/>
-      <c r="H135" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H135" s="7"/>
+      <c r="I135" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="136" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A136" s="7"/>
       <c r="B136" s="7"/>
       <c r="C136" s="7"/>
@@ -14605,11 +14749,12 @@
       <c r="E136" s="8"/>
       <c r="F136" s="7"/>
       <c r="G136" s="7"/>
-      <c r="H136" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H136" s="7"/>
+      <c r="I136" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="137" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A137" s="7"/>
       <c r="B137" s="7"/>
       <c r="C137" s="7"/>
@@ -14617,11 +14762,12 @@
       <c r="E137" s="8"/>
       <c r="F137" s="7"/>
       <c r="G137" s="7"/>
-      <c r="H137" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H137" s="7"/>
+      <c r="I137" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="138" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A138" s="7"/>
       <c r="B138" s="7"/>
       <c r="C138" s="7"/>
@@ -14629,11 +14775,12 @@
       <c r="E138" s="8"/>
       <c r="F138" s="7"/>
       <c r="G138" s="7"/>
-      <c r="H138" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H138" s="7"/>
+      <c r="I138" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="139" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A139" s="7"/>
       <c r="B139" s="7"/>
       <c r="C139" s="7"/>
@@ -14641,11 +14788,12 @@
       <c r="E139" s="8"/>
       <c r="F139" s="7"/>
       <c r="G139" s="7"/>
-      <c r="H139" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H139" s="7"/>
+      <c r="I139" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="140" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A140" s="7"/>
       <c r="B140" s="7"/>
       <c r="C140" s="7"/>
@@ -14653,11 +14801,12 @@
       <c r="E140" s="8"/>
       <c r="F140" s="7"/>
       <c r="G140" s="7"/>
-      <c r="H140" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H140" s="7"/>
+      <c r="I140" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="141" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A141" s="7"/>
       <c r="B141" s="7"/>
       <c r="C141" s="7"/>
@@ -14665,11 +14814,12 @@
       <c r="E141" s="8"/>
       <c r="F141" s="7"/>
       <c r="G141" s="7"/>
-      <c r="H141" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H141" s="7"/>
+      <c r="I141" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="142" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A142" s="7"/>
       <c r="B142" s="7"/>
       <c r="C142" s="7"/>
@@ -14677,11 +14827,12 @@
       <c r="E142" s="8"/>
       <c r="F142" s="7"/>
       <c r="G142" s="7"/>
-      <c r="H142" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H142" s="7"/>
+      <c r="I142" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="143" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A143" s="7"/>
       <c r="B143" s="7"/>
       <c r="C143" s="7"/>
@@ -14689,11 +14840,12 @@
       <c r="E143" s="8"/>
       <c r="F143" s="7"/>
       <c r="G143" s="7"/>
-      <c r="H143" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H143" s="7"/>
+      <c r="I143" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="144" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A144" s="7"/>
       <c r="B144" s="7"/>
       <c r="C144" s="7"/>
@@ -14701,11 +14853,12 @@
       <c r="E144" s="8"/>
       <c r="F144" s="7"/>
       <c r="G144" s="7"/>
-      <c r="H144" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H144" s="7"/>
+      <c r="I144" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="145" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A145" s="7"/>
       <c r="B145" s="7"/>
       <c r="C145" s="7"/>
@@ -14713,11 +14866,12 @@
       <c r="E145" s="8"/>
       <c r="F145" s="7"/>
       <c r="G145" s="7"/>
-      <c r="H145" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H145" s="7"/>
+      <c r="I145" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="146" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A146" s="7"/>
       <c r="B146" s="7"/>
       <c r="C146" s="7"/>
@@ -14725,11 +14879,12 @@
       <c r="E146" s="8"/>
       <c r="F146" s="7"/>
       <c r="G146" s="7"/>
-      <c r="H146" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H146" s="7"/>
+      <c r="I146" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="147" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A147" s="7"/>
       <c r="B147" s="7"/>
       <c r="C147" s="7"/>
@@ -14737,11 +14892,12 @@
       <c r="E147" s="8"/>
       <c r="F147" s="7"/>
       <c r="G147" s="7"/>
-      <c r="H147" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H147" s="7"/>
+      <c r="I147" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="148" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A148" s="7"/>
       <c r="B148" s="7"/>
       <c r="C148" s="7"/>
@@ -14749,11 +14905,12 @@
       <c r="E148" s="8"/>
       <c r="F148" s="7"/>
       <c r="G148" s="7"/>
-      <c r="H148" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H148" s="7"/>
+      <c r="I148" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="149" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A149" s="7"/>
       <c r="B149" s="7"/>
       <c r="C149" s="7"/>
@@ -14761,11 +14918,12 @@
       <c r="E149" s="8"/>
       <c r="F149" s="7"/>
       <c r="G149" s="7"/>
-      <c r="H149" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H149" s="7"/>
+      <c r="I149" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="150" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A150" s="7"/>
       <c r="B150" s="7"/>
       <c r="C150" s="7"/>
@@ -14773,11 +14931,12 @@
       <c r="E150" s="12"/>
       <c r="F150" s="7"/>
       <c r="G150" s="7"/>
-      <c r="H150" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H150" s="7"/>
+      <c r="I150" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="151" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A151" s="7"/>
       <c r="B151" s="7"/>
       <c r="C151" s="7"/>
@@ -14785,11 +14944,12 @@
       <c r="E151" s="8"/>
       <c r="F151" s="7"/>
       <c r="G151" s="7"/>
-      <c r="H151" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H151" s="7"/>
+      <c r="I151" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="152" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A152" s="7"/>
       <c r="B152" s="7"/>
       <c r="C152" s="7"/>
@@ -14797,11 +14957,12 @@
       <c r="E152" s="8"/>
       <c r="F152" s="7"/>
       <c r="G152" s="7"/>
-      <c r="H152" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H152" s="7"/>
+      <c r="I152" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="153" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A153" s="7"/>
       <c r="B153" s="7"/>
       <c r="C153" s="7"/>
@@ -14809,11 +14970,12 @@
       <c r="E153" s="8"/>
       <c r="F153" s="7"/>
       <c r="G153" s="7"/>
-      <c r="H153" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H153" s="7"/>
+      <c r="I153" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="154" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A154" s="7"/>
       <c r="B154" s="7"/>
       <c r="C154" s="7"/>
@@ -14821,11 +14983,12 @@
       <c r="E154" s="8"/>
       <c r="F154" s="7"/>
       <c r="G154" s="7"/>
-      <c r="H154" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H154" s="7"/>
+      <c r="I154" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="155" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A155" s="7"/>
       <c r="B155" s="7"/>
       <c r="C155" s="7"/>
@@ -14833,11 +14996,12 @@
       <c r="E155" s="8"/>
       <c r="F155" s="7"/>
       <c r="G155" s="7"/>
-      <c r="H155" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H155" s="7"/>
+      <c r="I155" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="156" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A156" s="7"/>
       <c r="B156" s="7"/>
       <c r="C156" s="7"/>
@@ -14845,11 +15009,12 @@
       <c r="E156" s="8"/>
       <c r="F156" s="7"/>
       <c r="G156" s="7"/>
-      <c r="H156" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H156" s="7"/>
+      <c r="I156" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="157" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A157" s="7"/>
       <c r="B157" s="7"/>
       <c r="C157" s="7"/>
@@ -14857,11 +15022,12 @@
       <c r="E157" s="8"/>
       <c r="F157" s="7"/>
       <c r="G157" s="7"/>
-      <c r="H157" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H157" s="7"/>
+      <c r="I157" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="158" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A158" s="7"/>
       <c r="B158" s="7"/>
       <c r="C158" s="7"/>
@@ -14869,11 +15035,12 @@
       <c r="E158" s="9"/>
       <c r="F158" s="7"/>
       <c r="G158" s="7"/>
-      <c r="H158" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H158" s="7"/>
+      <c r="I158" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="159" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A159" s="7"/>
       <c r="B159" s="7"/>
       <c r="C159" s="7"/>
@@ -14881,11 +15048,12 @@
       <c r="E159" s="8"/>
       <c r="F159" s="7"/>
       <c r="G159" s="7"/>
-      <c r="H159" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H159" s="7"/>
+      <c r="I159" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="160" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A160" s="7"/>
       <c r="B160" s="7"/>
       <c r="C160" s="7"/>
@@ -14893,11 +15061,12 @@
       <c r="E160" s="8"/>
       <c r="F160" s="7"/>
       <c r="G160" s="7"/>
-      <c r="H160" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H160" s="7"/>
+      <c r="I160" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="161" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A161" s="7"/>
       <c r="B161" s="1"/>
       <c r="C161" s="7"/>
@@ -14905,11 +15074,12 @@
       <c r="E161" s="8"/>
       <c r="F161" s="7"/>
       <c r="G161" s="7"/>
-      <c r="H161" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H161" s="7"/>
+      <c r="I161" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="162" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A162" s="7"/>
       <c r="B162" s="7"/>
       <c r="C162" s="7"/>
@@ -14917,11 +15087,12 @@
       <c r="E162" s="8"/>
       <c r="F162" s="7"/>
       <c r="G162" s="7"/>
-      <c r="H162" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H162" s="7"/>
+      <c r="I162" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="163" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A163" s="7"/>
       <c r="B163" s="7"/>
       <c r="C163" s="7"/>
@@ -14929,11 +15100,12 @@
       <c r="E163" s="8"/>
       <c r="F163" s="7"/>
       <c r="G163" s="7"/>
-      <c r="H163" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H163" s="7"/>
+      <c r="I163" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="164" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A164" s="7"/>
       <c r="B164" s="7"/>
       <c r="C164" s="7"/>
@@ -14941,11 +15113,12 @@
       <c r="E164" s="8"/>
       <c r="F164" s="7"/>
       <c r="G164" s="7"/>
-      <c r="H164" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H164" s="7"/>
+      <c r="I164" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="165" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A165" s="7"/>
       <c r="B165" s="7"/>
       <c r="C165" s="7"/>
@@ -14953,11 +15126,12 @@
       <c r="E165" s="8"/>
       <c r="F165" s="7"/>
       <c r="G165" s="7"/>
-      <c r="H165" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H165" s="7"/>
+      <c r="I165" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="166" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A166" s="7"/>
       <c r="B166" s="7"/>
       <c r="C166" s="7"/>
@@ -14965,11 +15139,12 @@
       <c r="E166" s="8"/>
       <c r="F166" s="7"/>
       <c r="G166" s="7"/>
-      <c r="H166" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H166" s="7"/>
+      <c r="I166" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="167" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A167" s="7"/>
       <c r="B167" s="7"/>
       <c r="C167" s="7"/>
@@ -14977,11 +15152,12 @@
       <c r="E167" s="12"/>
       <c r="F167" s="7"/>
       <c r="G167" s="7"/>
-      <c r="H167" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H167" s="7"/>
+      <c r="I167" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="168" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A168" s="7"/>
       <c r="B168" s="7"/>
       <c r="C168" s="7"/>
@@ -14989,11 +15165,12 @@
       <c r="E168" s="8"/>
       <c r="F168" s="7"/>
       <c r="G168" s="7"/>
-      <c r="H168" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H168" s="7"/>
+      <c r="I168" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="169" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A169" s="7"/>
       <c r="B169" s="7"/>
       <c r="C169" s="7"/>
@@ -15001,11 +15178,12 @@
       <c r="E169" s="8"/>
       <c r="F169" s="7"/>
       <c r="G169" s="7"/>
-      <c r="H169" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H169" s="7"/>
+      <c r="I169" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="170" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A170" s="7"/>
       <c r="B170" s="7"/>
       <c r="C170" s="7"/>
@@ -15013,11 +15191,12 @@
       <c r="E170" s="8"/>
       <c r="F170" s="7"/>
       <c r="G170" s="7"/>
-      <c r="H170" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H170" s="7"/>
+      <c r="I170" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="171" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A171" s="7"/>
       <c r="B171" s="7"/>
       <c r="C171" s="7"/>
@@ -15025,11 +15204,12 @@
       <c r="E171" s="8"/>
       <c r="F171" s="7"/>
       <c r="G171" s="7"/>
-      <c r="H171" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H171" s="7"/>
+      <c r="I171" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="172" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A172" s="7"/>
       <c r="B172" s="7"/>
       <c r="C172" s="7"/>
@@ -15037,11 +15217,12 @@
       <c r="E172" s="12"/>
       <c r="F172" s="7"/>
       <c r="G172" s="7"/>
-      <c r="H172" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="173" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H172" s="7"/>
+      <c r="I172" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="173" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A173" s="7"/>
       <c r="B173" s="7"/>
       <c r="C173" s="7"/>
@@ -15049,11 +15230,12 @@
       <c r="E173" s="12"/>
       <c r="F173" s="7"/>
       <c r="G173" s="7"/>
-      <c r="H173" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H173" s="7"/>
+      <c r="I173" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="174" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A174" s="7"/>
       <c r="B174" s="7"/>
       <c r="C174" s="7"/>
@@ -15061,11 +15243,12 @@
       <c r="E174" s="8"/>
       <c r="F174" s="7"/>
       <c r="G174" s="7"/>
-      <c r="H174" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H174" s="7"/>
+      <c r="I174" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="175" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A175" s="7"/>
       <c r="B175" s="7"/>
       <c r="C175" s="7"/>
@@ -15073,11 +15256,12 @@
       <c r="E175" s="8"/>
       <c r="F175" s="7"/>
       <c r="G175" s="7"/>
-      <c r="H175" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H175" s="7"/>
+      <c r="I175" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="176" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A176" s="7"/>
       <c r="B176" s="7"/>
       <c r="C176" s="7"/>
@@ -15085,11 +15269,12 @@
       <c r="E176" s="8"/>
       <c r="F176" s="7"/>
       <c r="G176" s="7"/>
-      <c r="H176" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="177" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H176" s="7"/>
+      <c r="I176" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="177" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A177" s="7"/>
       <c r="B177" s="7"/>
       <c r="C177" s="7"/>
@@ -15097,143 +15282,155 @@
       <c r="E177" s="8"/>
       <c r="F177" s="7"/>
       <c r="G177" s="7"/>
-      <c r="H177" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H177" s="7"/>
+      <c r="I177" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="178" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A178" s="7"/>
       <c r="B178" s="1"/>
       <c r="C178" s="1"/>
       <c r="D178" s="1"/>
       <c r="E178" s="3"/>
       <c r="F178" s="7"/>
-      <c r="G178" s="1"/>
-      <c r="H178" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="179" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G178" s="7"/>
+      <c r="H178" s="1"/>
+      <c r="I178" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="179" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A179" s="7"/>
       <c r="B179" s="1"/>
       <c r="C179" s="1"/>
       <c r="D179" s="1"/>
       <c r="E179" s="3"/>
       <c r="F179" s="7"/>
-      <c r="G179" s="1"/>
-      <c r="H179" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G179" s="7"/>
+      <c r="H179" s="1"/>
+      <c r="I179" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="180" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A180" s="7"/>
       <c r="B180" s="1"/>
       <c r="C180" s="1"/>
       <c r="D180" s="1"/>
       <c r="E180" s="3"/>
       <c r="F180" s="7"/>
-      <c r="G180" s="1"/>
-      <c r="H180" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="181" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G180" s="7"/>
+      <c r="H180" s="1"/>
+      <c r="I180" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="181" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A181" s="7"/>
       <c r="B181" s="1"/>
       <c r="C181" s="1"/>
       <c r="D181" s="1"/>
       <c r="E181" s="3"/>
       <c r="F181" s="7"/>
-      <c r="G181" s="1"/>
-      <c r="H181" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="182" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G181" s="7"/>
+      <c r="H181" s="1"/>
+      <c r="I181" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="182" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A182" s="7"/>
       <c r="B182" s="1"/>
       <c r="C182" s="1"/>
       <c r="D182" s="1"/>
       <c r="E182" s="3"/>
       <c r="F182" s="7"/>
-      <c r="G182" s="1"/>
-      <c r="H182" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="183" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G182" s="7"/>
+      <c r="H182" s="1"/>
+      <c r="I182" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="183" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A183" s="7"/>
       <c r="B183" s="1"/>
       <c r="C183" s="1"/>
       <c r="D183" s="1"/>
       <c r="E183" s="2"/>
       <c r="F183" s="7"/>
-      <c r="G183" s="1"/>
-      <c r="H183" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="184" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G183" s="7"/>
+      <c r="H183" s="1"/>
+      <c r="I183" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="184" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A184" s="1"/>
       <c r="B184" s="1"/>
       <c r="C184" s="1"/>
       <c r="D184" s="1"/>
       <c r="E184" s="3"/>
       <c r="F184" s="7"/>
-      <c r="G184" s="1"/>
-      <c r="H184" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="185" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G184" s="7"/>
+      <c r="H184" s="1"/>
+      <c r="I184" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="185" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A185" s="1"/>
       <c r="B185" s="1"/>
       <c r="C185" s="1"/>
       <c r="D185" s="1"/>
       <c r="E185" s="3"/>
       <c r="F185" s="7"/>
-      <c r="G185" s="1"/>
-      <c r="H185" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="186" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G185" s="7"/>
+      <c r="H185" s="1"/>
+      <c r="I185" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="186" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A186" s="1"/>
       <c r="B186" s="1"/>
       <c r="C186" s="1"/>
       <c r="D186" s="1"/>
       <c r="E186" s="3"/>
       <c r="F186" s="7"/>
-      <c r="G186" s="1"/>
-      <c r="H186" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="187" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G186" s="7"/>
+      <c r="H186" s="1"/>
+      <c r="I186" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="187" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A187" s="1"/>
       <c r="B187" s="1"/>
       <c r="C187" s="1"/>
       <c r="D187" s="1"/>
       <c r="E187" s="3"/>
       <c r="F187" s="7"/>
-      <c r="G187" s="1"/>
-      <c r="H187" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="188" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G187" s="7"/>
+      <c r="H187" s="1"/>
+      <c r="I187" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="188" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A188" s="1"/>
       <c r="B188" s="1"/>
       <c r="C188" s="1"/>
       <c r="D188" s="1"/>
       <c r="E188" s="3"/>
       <c r="F188" s="7"/>
-      <c r="G188" s="1"/>
-      <c r="H188" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="189" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G188" s="7"/>
+      <c r="H188" s="1"/>
+      <c r="I188" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="189" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A189" s="1"/>
       <c r="B189" s="1"/>
       <c r="C189" s="1"/>
@@ -15241,11 +15438,12 @@
       <c r="E189" s="3"/>
       <c r="F189" s="1"/>
       <c r="G189" s="1"/>
-      <c r="H189" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="190" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H189" s="1"/>
+      <c r="I189" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="190" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A190" s="1"/>
       <c r="B190" s="1"/>
       <c r="C190" s="1"/>
@@ -15253,11 +15451,12 @@
       <c r="E190" s="3"/>
       <c r="F190" s="1"/>
       <c r="G190" s="1"/>
-      <c r="H190" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="191" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H190" s="1"/>
+      <c r="I190" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="191" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A191" s="1"/>
       <c r="B191" s="1"/>
       <c r="C191" s="1"/>
@@ -15265,11 +15464,12 @@
       <c r="E191" s="2"/>
       <c r="F191" s="1"/>
       <c r="G191" s="1"/>
-      <c r="H191" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="192" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H191" s="1"/>
+      <c r="I191" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="192" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A192" s="1"/>
       <c r="B192" s="1"/>
       <c r="C192" s="1"/>
@@ -15277,11 +15477,12 @@
       <c r="E192" s="2"/>
       <c r="F192" s="1"/>
       <c r="G192" s="1"/>
-      <c r="H192" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="193" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H192" s="1"/>
+      <c r="I192" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="193" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A193" s="1"/>
       <c r="B193" s="1"/>
       <c r="C193" s="1"/>
@@ -15289,11 +15490,12 @@
       <c r="E193" s="2"/>
       <c r="F193" s="1"/>
       <c r="G193" s="1"/>
-      <c r="H193" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="194" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H193" s="1"/>
+      <c r="I193" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="194" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A194" s="1"/>
       <c r="B194" s="1"/>
       <c r="C194" s="1"/>
@@ -15301,11 +15503,12 @@
       <c r="E194" s="2"/>
       <c r="F194" s="1"/>
       <c r="G194" s="1"/>
-      <c r="H194" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="195" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H194" s="1"/>
+      <c r="I194" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="195" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A195" s="1"/>
       <c r="B195" s="1"/>
       <c r="C195" s="1"/>
@@ -15313,11 +15516,12 @@
       <c r="E195" s="2"/>
       <c r="F195" s="1"/>
       <c r="G195" s="1"/>
-      <c r="H195" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="196" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H195" s="1"/>
+      <c r="I195" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="196" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A196" s="1"/>
       <c r="B196" s="1"/>
       <c r="C196" s="1"/>
@@ -15325,11 +15529,12 @@
       <c r="E196" s="2"/>
       <c r="F196" s="1"/>
       <c r="G196" s="1"/>
-      <c r="H196" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="197" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H196" s="1"/>
+      <c r="I196" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="197" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A197" s="1"/>
       <c r="B197" s="1"/>
       <c r="C197" s="1"/>
@@ -15337,11 +15542,12 @@
       <c r="E197" s="2"/>
       <c r="F197" s="1"/>
       <c r="G197" s="1"/>
-      <c r="H197" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="198" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H197" s="1"/>
+      <c r="I197" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="198" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A198" s="1"/>
       <c r="B198" s="1"/>
       <c r="C198" s="1"/>
@@ -15349,11 +15555,12 @@
       <c r="E198" s="2"/>
       <c r="F198" s="1"/>
       <c r="G198" s="1"/>
-      <c r="H198" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="199" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H198" s="1"/>
+      <c r="I198" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="199" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A199" s="1"/>
       <c r="B199" s="1"/>
       <c r="C199" s="1"/>
@@ -15361,11 +15568,12 @@
       <c r="E199" s="2"/>
       <c r="F199" s="1"/>
       <c r="G199" s="1"/>
-      <c r="H199" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="200" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H199" s="1"/>
+      <c r="I199" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="200" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A200" s="1"/>
       <c r="B200" s="1"/>
       <c r="C200" s="1"/>
@@ -15373,11 +15581,12 @@
       <c r="E200" s="2"/>
       <c r="F200" s="1"/>
       <c r="G200" s="1"/>
-      <c r="H200" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="201" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H200" s="1"/>
+      <c r="I200" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="201" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A201" s="1"/>
       <c r="B201" s="1"/>
       <c r="C201" s="1"/>
@@ -15385,11 +15594,12 @@
       <c r="E201" s="2"/>
       <c r="F201" s="1"/>
       <c r="G201" s="1"/>
-      <c r="H201" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="202" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H201" s="1"/>
+      <c r="I201" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="202" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A202" s="1"/>
       <c r="B202" s="1"/>
       <c r="C202" s="1"/>
@@ -15397,11 +15607,12 @@
       <c r="E202" s="2"/>
       <c r="F202" s="1"/>
       <c r="G202" s="1"/>
-      <c r="H202" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="203" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H202" s="1"/>
+      <c r="I202" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="203" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A203" s="1"/>
       <c r="B203" s="1"/>
       <c r="C203" s="1"/>
@@ -15409,11 +15620,12 @@
       <c r="E203" s="2"/>
       <c r="F203" s="1"/>
       <c r="G203" s="1"/>
-      <c r="H203" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="204" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H203" s="1"/>
+      <c r="I203" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="204" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A204" s="1"/>
       <c r="B204" s="1"/>
       <c r="C204" s="1"/>
@@ -15421,11 +15633,12 @@
       <c r="E204" s="2"/>
       <c r="F204" s="1"/>
       <c r="G204" s="1"/>
-      <c r="H204" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="205" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H204" s="1"/>
+      <c r="I204" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="205" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A205" s="1"/>
       <c r="B205" s="1"/>
       <c r="C205" s="1"/>
@@ -15433,11 +15646,12 @@
       <c r="E205" s="2"/>
       <c r="F205" s="1"/>
       <c r="G205" s="1"/>
-      <c r="H205" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="206" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H205" s="1"/>
+      <c r="I205" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="206" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A206" s="1"/>
       <c r="B206" s="1"/>
       <c r="C206" s="1"/>
@@ -15445,11 +15659,12 @@
       <c r="E206" s="2"/>
       <c r="F206" s="1"/>
       <c r="G206" s="1"/>
-      <c r="H206" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="207" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H206" s="1"/>
+      <c r="I206" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="207" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A207" s="1"/>
       <c r="B207" s="1"/>
       <c r="C207" s="1"/>
@@ -15457,11 +15672,12 @@
       <c r="E207" s="2"/>
       <c r="F207" s="1"/>
       <c r="G207" s="1"/>
-      <c r="H207" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="208" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H207" s="1"/>
+      <c r="I207" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="208" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A208" s="1"/>
       <c r="B208" s="1"/>
       <c r="C208" s="1"/>
@@ -15469,11 +15685,12 @@
       <c r="E208" s="2"/>
       <c r="F208" s="1"/>
       <c r="G208" s="1"/>
-      <c r="H208" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="209" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H208" s="1"/>
+      <c r="I208" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="209" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A209" s="1"/>
       <c r="B209" s="1"/>
       <c r="C209" s="1"/>
@@ -15481,11 +15698,12 @@
       <c r="E209" s="2"/>
       <c r="F209" s="1"/>
       <c r="G209" s="1"/>
-      <c r="H209" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="210" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H209" s="1"/>
+      <c r="I209" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="210" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A210" s="1"/>
       <c r="B210" s="1"/>
       <c r="C210" s="1"/>
@@ -15493,11 +15711,12 @@
       <c r="E210" s="2"/>
       <c r="F210" s="1"/>
       <c r="G210" s="1"/>
-      <c r="H210" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="211" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H210" s="1"/>
+      <c r="I210" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="211" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A211" s="1"/>
       <c r="B211" s="1"/>
       <c r="C211" s="1"/>
@@ -15505,7 +15724,8 @@
       <c r="E211" s="2"/>
       <c r="F211" s="1"/>
       <c r="G211" s="1"/>
-      <c r="H211" s="1" t="s">
+      <c r="H211" s="1"/>
+      <c r="I211" s="1" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>